<commit_message>
Add dev and prod profiles with H2 database configuration; enhance Swagger documentation
</commit_message>
<xml_diff>
--- a/posts_report.xlsx
+++ b/posts_report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -26,10 +26,10 @@
     <t>Created At</t>
   </si>
   <si>
-    <t>фцвфцв</t>
-  </si>
-  <si>
-    <t>фцвфвц</t>
+    <t>фцвфцвawdawd</t>
+  </si>
+  <si>
+    <t>фцвфвцww</t>
   </si>
   <si>
     <t>2024-12-11T16:00:13.090677</t>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>2024-12-11T16:06:09.528828</t>
+  </si>
+  <si>
+    <t>awd</t>
+  </si>
+  <si>
+    <t>2024-12-11T16:08:57.782325</t>
+  </si>
+  <si>
+    <t>ыуаыуа</t>
+  </si>
+  <si>
+    <t>2024-12-11T16:21:41.180195</t>
   </si>
 </sst>
 </file>
@@ -95,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -157,6 +169,34 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>